<commit_message>
stroke units ch gps data
</commit_message>
<xml_diff>
--- a/daten/stroke_units_ch.xlsx
+++ b/daten/stroke_units_ch.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3a87f39a522517ac/FHGR/4. Semester/Masterthesis/Daten/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/laurazanchin/Dropbox/Mac/Desktop/master/daten/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="104" documentId="8_{E1F5AE2F-4A0B-DE4F-9B0C-84A07E1B92B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FB727DAE-DD32-E344-BD06-EDBBD49828AC}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EE423EA-D5B5-034D-8743-64D788D8DD39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3480" yWindow="2600" windowWidth="27440" windowHeight="16240" xr2:uid="{703E470E-EBFD-0D4E-94A4-7298E40D5768}"/>
+    <workbookView xWindow="10580" yWindow="1280" windowWidth="27440" windowHeight="16240" xr2:uid="{703E470E-EBFD-0D4E-94A4-7298E40D5768}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="77">
   <si>
     <t>Klinik</t>
   </si>
@@ -50,9 +50,6 @@
     <t>Ort</t>
   </si>
   <si>
-    <t>Anzahl</t>
-  </si>
-  <si>
     <t>Hôpital Neuchâtelois</t>
   </si>
   <si>
@@ -74,9 +71,6 @@
     <t>HFR Fribourg Hôpital Cantonal</t>
   </si>
   <si>
-    <t>Kantonsspital Baden  </t>
-  </si>
-  <si>
     <t>Bürgerspital Solothurn</t>
   </si>
   <si>
@@ -101,9 +95,6 @@
     <t>Neuchâtel</t>
   </si>
   <si>
-    <t>Av. Grand-Champsec 80</t>
-  </si>
-  <si>
     <t>Sion</t>
   </si>
   <si>
@@ -134,9 +125,6 @@
     <t>Schlieren</t>
   </si>
   <si>
-    <t>Chem. des Pensionnats 2/6</t>
-  </si>
-  <si>
     <t>Villars-sur-Glâne</t>
   </si>
   <si>
@@ -176,18 +164,125 @@
     <t>Nyon</t>
   </si>
   <si>
-    <t>Stroke Units Schweiz</t>
-  </si>
-  <si>
     <t>Maladière 45</t>
+  </si>
+  <si>
+    <t>Kantonsspital St. Gallen</t>
+  </si>
+  <si>
+    <t>Rorschacher Strasse 95</t>
+  </si>
+  <si>
+    <t>St. Gallen</t>
+  </si>
+  <si>
+    <t>Kantonsspital Aarau</t>
+  </si>
+  <si>
+    <t>Tellstrasse 25</t>
+  </si>
+  <si>
+    <t>Aarau</t>
+  </si>
+  <si>
+    <t>HUG, Hôpitaux Universitaires Genève</t>
+  </si>
+  <si>
+    <t>Rue Gabrielle-Perret-Gentil 4</t>
+  </si>
+  <si>
+    <t>Genf</t>
+  </si>
+  <si>
+    <t>Inselspital Bern</t>
+  </si>
+  <si>
+    <t>Freiburgstrasse 16</t>
+  </si>
+  <si>
+    <t>Bern</t>
+  </si>
+  <si>
+    <t>CHUV, Lausanne</t>
+  </si>
+  <si>
+    <t>Rue du Bugnon 46</t>
+  </si>
+  <si>
+    <t>Lausanne</t>
+  </si>
+  <si>
+    <t>EOC, Ospedale Regionale di Lugano (Civico)</t>
+  </si>
+  <si>
+    <t>Via Tesserete 46</t>
+  </si>
+  <si>
+    <t>Lugano</t>
+  </si>
+  <si>
+    <t>USB, Universitätsspital Basel</t>
+  </si>
+  <si>
+    <t>Petersgraben 4</t>
+  </si>
+  <si>
+    <t>Basel</t>
+  </si>
+  <si>
+    <t>Universitätsspital Zürich</t>
+  </si>
+  <si>
+    <t>Frauenklinikstrasse 26</t>
+  </si>
+  <si>
+    <t>Hirslanden Zürich</t>
+  </si>
+  <si>
+    <t>Witellikerstrasse 40</t>
+  </si>
+  <si>
+    <t>Luzerner Kantonsspital</t>
+  </si>
+  <si>
+    <t>Spitalstrasse 16</t>
+  </si>
+  <si>
+    <t>Luzern</t>
+  </si>
+  <si>
+    <t>stroke_centers</t>
+  </si>
+  <si>
+    <t>stroke_units</t>
+  </si>
+  <si>
+    <t>Kategorie</t>
+  </si>
+  <si>
+    <t>Kantonsspital Baden</t>
+  </si>
+  <si>
+    <t>Chemin des Pensionnats 2</t>
+  </si>
+  <si>
+    <t>Avenue Grand-Champsec 80</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -215,8 +310,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -232,10 +328,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -535,289 +627,455 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA90C6D4-C3FC-C54A-AA8E-1FD120BC0EAE}">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.83203125" customWidth="1"/>
-    <col min="2" max="2" width="32" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>46</v>
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2">
+        <v>2000</v>
+      </c>
+      <c r="D2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="B3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" t="s">
-        <v>1</v>
+        <v>76</v>
+      </c>
+      <c r="C3">
+        <v>1950</v>
       </c>
       <c r="D3" t="s">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="E3" t="s">
-        <v>3</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>1</v>
+      <c r="A4" t="s">
+        <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4">
+        <v>8063</v>
+      </c>
+      <c r="D4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5">
+        <v>2502</v>
+      </c>
+      <c r="D5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6">
+        <v>9472</v>
+      </c>
+      <c r="D6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7">
+        <v>8401</v>
+      </c>
+      <c r="D7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8">
+        <v>8952</v>
+      </c>
+      <c r="D8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" t="s">
+        <v>75</v>
+      </c>
+      <c r="C9">
+        <v>1752</v>
+      </c>
+      <c r="D9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>74</v>
+      </c>
+      <c r="B10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10">
+        <v>5404</v>
+      </c>
+      <c r="D10" t="s">
+        <v>31</v>
+      </c>
+      <c r="E10" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11">
+        <v>4500</v>
+      </c>
+      <c r="D11" t="s">
+        <v>33</v>
+      </c>
+      <c r="E11" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12">
+        <v>8596</v>
+      </c>
+      <c r="D12" t="s">
+        <v>35</v>
+      </c>
+      <c r="E12" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13">
+        <v>7000</v>
+      </c>
+      <c r="D13" t="s">
+        <v>37</v>
+      </c>
+      <c r="E13" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14">
+        <v>1269</v>
+      </c>
+      <c r="D14" t="s">
+        <v>41</v>
+      </c>
+      <c r="E14" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15">
+        <v>8501</v>
+      </c>
+      <c r="D15" t="s">
+        <v>39</v>
+      </c>
+      <c r="E15" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16" t="s">
+        <v>44</v>
+      </c>
+      <c r="C16">
+        <v>9007</v>
+      </c>
+      <c r="D16" t="s">
+        <v>45</v>
+      </c>
+      <c r="E16" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>46</v>
+      </c>
+      <c r="B17" t="s">
         <v>47</v>
       </c>
-      <c r="D4">
-        <v>2000</v>
-      </c>
-      <c r="E4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>2</v>
-      </c>
-      <c r="B5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5">
-        <v>1950</v>
-      </c>
-      <c r="E5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>3</v>
-      </c>
-      <c r="B6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6">
-        <v>8063</v>
-      </c>
-      <c r="E6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>4</v>
-      </c>
-      <c r="B7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" t="s">
-        <v>24</v>
-      </c>
-      <c r="D7">
-        <v>2502</v>
-      </c>
-      <c r="E7" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>5</v>
-      </c>
-      <c r="B8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" t="s">
-        <v>26</v>
-      </c>
-      <c r="D8">
-        <v>9472</v>
-      </c>
-      <c r="E8" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>6</v>
-      </c>
-      <c r="B9" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" t="s">
-        <v>28</v>
-      </c>
-      <c r="D9">
-        <v>8401</v>
-      </c>
-      <c r="E9" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10">
-        <v>7</v>
-      </c>
-      <c r="B10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" t="s">
-        <v>30</v>
-      </c>
-      <c r="D10">
-        <v>8952</v>
-      </c>
-      <c r="E10" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11">
-        <v>8</v>
-      </c>
-      <c r="B11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" t="s">
-        <v>32</v>
-      </c>
-      <c r="D11">
-        <v>1752</v>
-      </c>
-      <c r="E11" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12">
-        <v>9</v>
-      </c>
-      <c r="B12" t="s">
-        <v>12</v>
-      </c>
-      <c r="C12" t="s">
-        <v>34</v>
-      </c>
-      <c r="D12">
-        <v>5404</v>
-      </c>
-      <c r="E12" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13">
-        <v>10</v>
-      </c>
-      <c r="B13" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" t="s">
-        <v>36</v>
-      </c>
-      <c r="D13">
-        <v>4500</v>
-      </c>
-      <c r="E13" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14">
-        <v>11</v>
-      </c>
-      <c r="B14" t="s">
-        <v>14</v>
-      </c>
-      <c r="C14" t="s">
-        <v>38</v>
-      </c>
-      <c r="D14">
-        <v>8596</v>
-      </c>
-      <c r="E14" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15">
-        <v>12</v>
-      </c>
-      <c r="B15" t="s">
-        <v>15</v>
-      </c>
-      <c r="C15" t="s">
-        <v>40</v>
-      </c>
-      <c r="D15">
-        <v>7000</v>
-      </c>
-      <c r="E15" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16">
-        <v>13</v>
-      </c>
-      <c r="B16" t="s">
-        <v>16</v>
-      </c>
-      <c r="C16" t="s">
-        <v>44</v>
-      </c>
-      <c r="D16">
-        <v>1269</v>
-      </c>
-      <c r="E16" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17">
-        <v>14</v>
-      </c>
-      <c r="B17" t="s">
+      <c r="C17">
+        <v>5001</v>
+      </c>
+      <c r="D17" t="s">
+        <v>48</v>
+      </c>
+      <c r="E17" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>49</v>
+      </c>
+      <c r="B18" t="s">
+        <v>50</v>
+      </c>
+      <c r="C18">
+        <v>1205</v>
+      </c>
+      <c r="D18" t="s">
+        <v>51</v>
+      </c>
+      <c r="E18" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>52</v>
+      </c>
+      <c r="B19" t="s">
+        <v>53</v>
+      </c>
+      <c r="C19">
+        <v>3010</v>
+      </c>
+      <c r="D19" t="s">
+        <v>54</v>
+      </c>
+      <c r="E19" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>55</v>
+      </c>
+      <c r="B20" t="s">
+        <v>56</v>
+      </c>
+      <c r="C20">
+        <v>1011</v>
+      </c>
+      <c r="D20" t="s">
+        <v>57</v>
+      </c>
+      <c r="E20" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>58</v>
+      </c>
+      <c r="B21" t="s">
+        <v>59</v>
+      </c>
+      <c r="C21">
+        <v>6900</v>
+      </c>
+      <c r="D21" t="s">
+        <v>60</v>
+      </c>
+      <c r="E21" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>61</v>
+      </c>
+      <c r="B22" t="s">
+        <v>62</v>
+      </c>
+      <c r="C22">
+        <v>4031</v>
+      </c>
+      <c r="D22" t="s">
+        <v>63</v>
+      </c>
+      <c r="E22" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>64</v>
+      </c>
+      <c r="B23" t="s">
+        <v>65</v>
+      </c>
+      <c r="C23">
+        <v>8091</v>
+      </c>
+      <c r="D23" t="s">
         <v>17</v>
       </c>
-      <c r="C17" t="s">
-        <v>42</v>
-      </c>
-      <c r="D17">
-        <v>8501</v>
-      </c>
-      <c r="E17" t="s">
-        <v>43</v>
+      <c r="E23" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>66</v>
+      </c>
+      <c r="B24" t="s">
+        <v>67</v>
+      </c>
+      <c r="C24">
+        <v>8032</v>
+      </c>
+      <c r="D24" t="s">
+        <v>17</v>
+      </c>
+      <c r="E24" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>68</v>
+      </c>
+      <c r="B25" t="s">
+        <v>69</v>
+      </c>
+      <c r="C25">
+        <v>6000</v>
+      </c>
+      <c r="D25" t="s">
+        <v>70</v>
+      </c>
+      <c r="E25" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B7" r:id="rId1" display="http://www.spitalzentrum-biel.ch/unternehmen/qualitaet/zertifizierungen/" xr:uid="{EA2F3978-6E83-DE45-8853-9C7215ED7EC3}"/>
-    <hyperlink ref="B17" r:id="rId2" tooltip="Opens internal link in current window" display="https://www.stgag.ch/fachbereiche/kliniken-fuer-innere-medizin/klinik-fuer-innere-medizin-am-kantonsspital-muensterlingen/neurologie/stroke-unit-schlaganfalleinheit-1/" xr:uid="{332D7D33-B952-694F-A671-165EA6BFB280}"/>
-    <hyperlink ref="B16" r:id="rId3" display="http://www.ghol.ch/jcms/ghol_6844/fr/unite-neurovasculaire-stroke-unit" xr:uid="{B9606763-2475-2E4F-9295-FFF113FD846D}"/>
-    <hyperlink ref="B15" r:id="rId4" display="https://www.so-h.ch/buergerspital-solothurn/home.html" xr:uid="{259CD451-8E03-6149-9A35-A642884737A8}"/>
-    <hyperlink ref="B14" r:id="rId5" display="https://www.so-h.ch/buergerspital-solothurn/home.html" xr:uid="{D27A27FC-5DE7-9642-BF48-4A913A636AB8}"/>
-    <hyperlink ref="B13" r:id="rId6" display="https://www.so-h.ch/buergerspital-solothurn/home.html" xr:uid="{871ECD03-0532-B844-A9E2-74D3456AA709}"/>
-    <hyperlink ref="B12" r:id="rId7" display="http://www.kantonsspitalbaden.ch/Fachbereiche/Stroke-Unit/index.html" xr:uid="{8541639D-DC4A-0944-956B-FF36FB3E4F68}"/>
-    <hyperlink ref="B11" r:id="rId8" display="http://www.h-fr.ch/hfr/fr/pub/metanav/lang.htm" xr:uid="{D571C6F8-68C5-8944-A524-8BFB41E58310}"/>
-    <hyperlink ref="B9" r:id="rId9" display="http://www.ksw.ch/desktopdefault.aspx/tabid-1876" xr:uid="{8394B474-41B0-7042-91E0-06605D584904}"/>
+    <hyperlink ref="A5" r:id="rId1" display="http://www.spitalzentrum-biel.ch/unternehmen/qualitaet/zertifizierungen/" xr:uid="{EA2F3978-6E83-DE45-8853-9C7215ED7EC3}"/>
+    <hyperlink ref="A15" r:id="rId2" tooltip="Opens internal link in current window" display="https://www.stgag.ch/fachbereiche/kliniken-fuer-innere-medizin/klinik-fuer-innere-medizin-am-kantonsspital-muensterlingen/neurologie/stroke-unit-schlaganfalleinheit-1/" xr:uid="{332D7D33-B952-694F-A671-165EA6BFB280}"/>
+    <hyperlink ref="A14" r:id="rId3" display="http://www.ghol.ch/jcms/ghol_6844/fr/unite-neurovasculaire-stroke-unit" xr:uid="{B9606763-2475-2E4F-9295-FFF113FD846D}"/>
+    <hyperlink ref="A13" r:id="rId4" display="https://www.so-h.ch/buergerspital-solothurn/home.html" xr:uid="{259CD451-8E03-6149-9A35-A642884737A8}"/>
+    <hyperlink ref="A12" r:id="rId5" display="https://www.so-h.ch/buergerspital-solothurn/home.html" xr:uid="{D27A27FC-5DE7-9642-BF48-4A913A636AB8}"/>
+    <hyperlink ref="A11" r:id="rId6" display="https://www.so-h.ch/buergerspital-solothurn/home.html" xr:uid="{871ECD03-0532-B844-A9E2-74D3456AA709}"/>
+    <hyperlink ref="A10" r:id="rId7" display="http://www.kantonsspitalbaden.ch/Fachbereiche/Stroke-Unit/index.html" xr:uid="{8541639D-DC4A-0944-956B-FF36FB3E4F68}"/>
+    <hyperlink ref="A9" r:id="rId8" display="http://www.h-fr.ch/hfr/fr/pub/metanav/lang.htm" xr:uid="{D571C6F8-68C5-8944-A524-8BFB41E58310}"/>
+    <hyperlink ref="A7" r:id="rId9" display="http://www.ksw.ch/desktopdefault.aspx/tabid-1876" xr:uid="{8394B474-41B0-7042-91E0-06605D584904}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>